<commit_message>
update to use at CC
</commit_message>
<xml_diff>
--- a/notebookscc/ana_summer2021/logbooks/auxtelholologbook_2021_07_07_v3.0.xlsx
+++ b/notebookscc/ana_summer2021/logbooks/auxtelholologbook_2021_07_07_v3.0.xlsx
@@ -457,7 +457,7 @@
     <t>2021-07-08T05:14:50.080</t>
   </si>
   <si>
-    <t>/Users/dagoret/DATA/AuxTelData2021/holo/quickLookExp/2021-07-07</t>
+    <t>/sps/lsst/groups/auxtel/data/2021/holo/quickLookExp/2021-07-07</t>
   </si>
   <si>
     <t>holo4_003_RG610_HD160617_20210707_000234_quickLookExp.fits</t>
@@ -6920,8 +6920,20 @@
       <c r="Q98">
         <v>6.8</v>
       </c>
+      <c r="R98">
+        <v>300</v>
+      </c>
+      <c r="S98">
+        <v>1600</v>
+      </c>
       <c r="V98" t="s">
         <v>276</v>
+      </c>
+      <c r="W98">
+        <v>1</v>
+      </c>
+      <c r="X98">
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:24">

</xml_diff>